<commit_message>
Ejay 2025May07-19:07 RATA TUR JV Reversal + fixes
</commit_message>
<xml_diff>
--- a/assets/templates/jv_reversal_template.xlsx
+++ b/assets/templates/jv_reversal_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.LAPTOP-3C0I7G4T\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.LAPTOP-3C0I7G4T\Projects\rata_backend-1\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19226CB1-1F83-4CD7-9DB0-4DE7C23C9665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6AEBDF-6FA2-434B-B381-F708307FC215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{30AEFB1A-8ABB-4EBA-B3E4-E86F68D12C62}"/>
   </bookViews>
@@ -197,18 +197,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -224,16 +215,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -549,9 +538,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21A4120-9680-4D7F-A09D-3CA9A96B9176}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -573,363 +562,260 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
     </row>
     <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="K14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="L14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="12" t="s">
+      <c r="M14" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="16"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="16"/>
-    </row>
-    <row r="17" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="16"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="16"/>
-    </row>
-    <row r="19" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="21" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="13"/>
-    </row>
-    <row r="22" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="13"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="13"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>